<commit_message>
cosine similarity, job API call
</commit_message>
<xml_diff>
--- a/ResumeSite/webapp/Extracted Data/Extracted.xlsx
+++ b/ResumeSite/webapp/Extracted Data/Extracted.xlsx
@@ -1,24 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-02-24" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-02-23" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-10-30" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-10-22" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-10-21" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-10-19" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-10-16" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-10-04" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-09-01" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-08-31" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-08-29" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="2024-04-04" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="2024-03-15" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="2024-03-14" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="2024-02-24" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="2024-02-23" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="2023-10-30" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="2023-10-22" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="2023-10-21" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="2023-10-19" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="2023-10-16" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="2023-10-04" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="2023-09-01" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="2023-08-31" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="2023-08-29" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Sheet" sheetId="15" state="visible" r:id="rId15"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -424,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,136 +455,374 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>thaleavanti2002@gmail.com</t>
+          <t>mrunalkulkarni.2802@gmail.com</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>+918605131403</t>
+          <t>7715027944</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>C, Analytics, Database, Python, Engineering, Matplotlib, Java, Github, Access, Website, Javascript, Nltk, Django, Analysis, Training, Php, Css, Programming, Jupyter, Spacy, Numpy, Sql, Pandas, System, Algorithms, Html, Mysql, Technical, Testing, Seaborn</t>
+          <t>Analysis, Communication, Queries, Content, Engineering, Technical, Ai, Nltk, Html, Numpy, Tensorflow, Design, Analytics, Programming, Django, C, Mysql, Certification, Pandas, Testing, Matplotlib, System, C++, Sql, Reports, Jupyter, Logbook, Networking, Php, Process, Rest, Javascript, Api, Website, Apis, Database, Python, Training, Css, Research</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>thaleavanti2002@gmail.com</t>
+          <t>mrunalkulkarni.2802@gmail.com</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>+918605131403</t>
+          <t>7715027944</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>C, Analytics, Database, Python, Engineering, Matplotlib, Java, Github, Access, Website, Javascript, Nltk, Django, Analysis, Training, Php, Css, Programming, Jupyter, Spacy, Numpy, Sql, Pandas, System, Algorithms, Html, Mysql, Technical, Testing, Seaborn</t>
+          <t>Analysis, Communication, Queries, Content, Engineering, Technical, Ai, Nltk, Html, Numpy, Tensorflow, Design, Analytics, Programming, Django, C, Mysql, Certification, Pandas, Testing, Matplotlib, System, C++, Sql, Reports, Jupyter, Logbook, Networking, Php, Process, Rest, Javascript, Api, Website, Apis, Database, Python, Training, Css, Research</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>thaleavanti2002@gmail.com</t>
+          <t>mrunalkulkarni.2802@gmail.com</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>+918605131403</t>
+          <t>7715027944</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>C, Analytics, Database, Python, Engineering, Matplotlib, Java, Github, Access, Website, Javascript, Nltk, Django, Analysis, Training, Php, Css, Programming, Jupyter, Spacy, Numpy, Sql, Pandas, System, Algorithms, Html, Mysql, Technical, Testing, Seaborn</t>
+          <t>Pandas, Javascript, Research, Tensorflow, Networking, Analytics, C, Technical, Mysql, Engineering, Content, Matplotlib, Api, C++, Html, Jupyter, Certification, Logbook, Website, Ai, Design, System, Css, Apis, Process, Database, Php, Analysis, Testing, Queries, Reports, Django, Python, Rest, Sql, Programming, Training, Numpy, Communication, Nltk</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>thaleavanti2002@gmail.com</t>
+          <t>mrunalkulkarni.2802@gmail.com</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>+918605131403</t>
+          <t>7715027944</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Programming, Nltk, Java, Engineering, Database, Php, Sql, Jupyter, Javascript, Website, Django, Analytics, Spacy, Seaborn, Css, System, Html, Analysis, C, Python, Pandas, Access, Mysql, Algorithms, Technical, Matplotlib, Github, Testing, Numpy, Training</t>
+          <t>Pandas, Javascript, Research, Tensorflow, Networking, Analytics, C, Technical, Mysql, Engineering, Content, Matplotlib, Api, C++, Html, Jupyter, Certification, Logbook, Website, Ai, Design, System, Css, Apis, Process, Database, Php, Analysis, Testing, Queries, Reports, Django, Python, Rest, Sql, Programming, Training, Numpy, Communication, Nltk</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>thaleavanti2002@gmail.com</t>
+          <t>mrunalkulkarni.2802@gmail.com</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>+918605131403</t>
+          <t>7715027944</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Programming, Nltk, Java, Engineering, Database, Php, Sql, Jupyter, Javascript, Website, Django, Analytics, Spacy, Seaborn, Css, System, Html, Analysis, C, Python, Pandas, Access, Mysql, Algorithms, Technical, Matplotlib, Github, Testing, Numpy, Training</t>
+          <t>Pandas, Javascript, Research, Tensorflow, Networking, Analytics, C, Technical, Mysql, Engineering, Content, Matplotlib, Api, C++, Html, Jupyter, Certification, Logbook, Website, Ai, Design, System, Css, Apis, Process, Database, Php, Analysis, Testing, Queries, Reports, Django, Python, Rest, Sql, Programming, Training, Numpy, Communication, Nltk</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>thaleavanti2002@gmail.com</t>
+          <t>mrunalkulkarni.2802@gmail.com</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>+918605131403</t>
+          <t>7715027944</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Programming, Nltk, Java, Engineering, Database, Php, Sql, Jupyter, Javascript, Website, Django, Analytics, Spacy, Seaborn, Css, System, Html, Analysis, C, Python, Pandas, Access, Mysql, Algorithms, Technical, Matplotlib, Github, Testing, Numpy, Training</t>
+          <t>Pandas, Javascript, Research, Tensorflow, Networking, Analytics, C, Technical, Mysql, Engineering, Content, Matplotlib, Api, C++, Html, Jupyter, Certification, Logbook, Website, Ai, Design, System, Css, Apis, Process, Database, Php, Analysis, Testing, Queries, Reports, Django, Python, Rest, Sql, Programming, Training, Numpy, Communication, Nltk</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>thaleavanti2002@gmail.com</t>
+          <t>mrunalkulkarni.2802@gmail.com</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>+918605131403</t>
+          <t>7715027944</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Programming, Nltk, Java, Engineering, Database, Php, Sql, Jupyter, Javascript, Website, Django, Analytics, Spacy, Seaborn, Css, System, Html, Analysis, C, Python, Pandas, Access, Mysql, Algorithms, Technical, Matplotlib, Github, Testing, Numpy, Training</t>
+          <t>Programming, Networking, Sql, Matplotlib, Rest, Website, Css, C++, Testing, Tensorflow, Ai, Database, Reports, Jupyter, Certification, Queries, Python, C, Php, Pandas, Training, Numpy, Html, Technical, Research, Analysis, Engineering, Django, Content, Mysql, Communication, System, Analytics, Nltk, Logbook, Design, Javascript, Api, Process, Apis</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>thaleavanti2002@gmail.com</t>
+          <t>mrunalkulkarni.2802@gmail.com</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>+918605131403</t>
+          <t>7715027944</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Programming, Nltk, Java, Engineering, Database, Php, Sql, Jupyter, Javascript, Website, Django, Analytics, Spacy, Seaborn, Css, System, Html, Analysis, C, Python, Pandas, Access, Mysql, Algorithms, Technical, Matplotlib, Github, Testing, Numpy, Training</t>
+          <t>Programming, Networking, Sql, Matplotlib, Rest, Website, Css, C++, Testing, Tensorflow, Ai, Database, Reports, Jupyter, Certification, Queries, Python, C, Php, Pandas, Training, Numpy, Html, Technical, Research, Analysis, Engineering, Django, Content, Mysql, Communication, System, Analytics, Nltk, Logbook, Design, Javascript, Api, Process, Apis</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Programming, Networking, Sql, Matplotlib, Rest, Website, Css, C++, Testing, Tensorflow, Ai, Database, Reports, Jupyter, Certification, Queries, Python, C, Php, Pandas, Training, Numpy, Html, Technical, Research, Analysis, Engineering, Django, Content, Mysql, Communication, System, Analytics, Nltk, Logbook, Design, Javascript, Api, Process, Apis</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Programming, Networking, Sql, Matplotlib, Rest, Website, Css, C++, Testing, Tensorflow, Ai, Database, Reports, Jupyter, Certification, Queries, Python, C, Php, Pandas, Training, Numpy, Html, Technical, Research, Analysis, Engineering, Django, Content, Mysql, Communication, System, Analytics, Nltk, Logbook, Design, Javascript, Api, Process, Apis</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Content, Testing, Reports, Python, Matplotlib, Ai, System, Mysql, C, Jupyter, Website, Django, Rest, Pandas, C++, Technical, Html, Process, Certification, Analysis, Nltk, Engineering, Logbook, Database, Apis, Design, Networking, Programming, Research, Queries, Tensorflow, Training, Php, Communication, Css, Analytics, Api, Numpy, Sql, Javascript</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Content, Reports, Warehouse, Python, Matplotlib, Mysql, Jupyter, C, Website, Pandas, C++, Technical, Html, Process, Certification, Spacy, Analysis, Nltk, Engineering, Logbook, Database, Design, Networking, Mining, Programming, Research, Queries, Tensorflow, Training, Php, Analytics, Css, Numpy, Sql, Javascript</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Mysql, Python, Javascript, Pandas, Reports, Jupyter, Analytics, Tensorflow, Research, Engineering, Analysis, C++, Php, Numpy, Certification, Networking, Database, Mining, Spacy, Warehouse, Sql, Programming, Html, Css, Logbook, Matplotlib, C, Process, Design, Website, Nltk, Content, Training, Queries, Technical</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Mysql, Python, Javascript, Pandas, Reports, Jupyter, Analytics, Tensorflow, Research, Engineering, Analysis, C++, Php, Numpy, Certification, Networking, Database, Mining, Spacy, Warehouse, Sql, Programming, Html, Css, Logbook, Matplotlib, C, Process, Design, Website, Nltk, Content, Training, Queries, Technical</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Html, Php, Python, Queries, Nltk, Tensorflow, Website, Sql, C++, Logbook, Database, Javascript, Warehouse, Analysis, Process, Spacy, Training, Engineering, Matplotlib, Design, Jupyter, Technical, Numpy, Reports, Pandas, Css, Programming, Mysql, Research, Mining, Content, Analytics, Networking, C, Certification</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Html, Php, Python, Queries, Nltk, Tensorflow, Website, Sql, C++, Logbook, Database, Javascript, Warehouse, Analysis, Process, Spacy, Training, Engineering, Matplotlib, Design, Jupyter, Technical, Numpy, Reports, Pandas, Css, Programming, Mysql, Research, Mining, Content, Analytics, Networking, C, Certification</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Html, Php, Python, Queries, Testing, Nltk, Ai, Tensorflow, Website, Sql, Rest, C++, Logbook, Database, Javascript, Analysis, Process, Engineering, Matplotlib, Django, Training, Design, Jupyter, Technical, Numpy, Communication, Reports, Apis, Pandas, Css, Programming, Mysql, Research, Content, Api, Analytics, Networking, System, C, Certification</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Networking, Html, Css, Database, Javascript, Website, Numpy, Apis, Reports, Research, Engineering, System, Rest, Testing, Communication, Sql, Matplotlib, Mysql, Analytics, C, Tensorflow, Pandas, Logbook, Content, Process, Design, Analysis, Technical, Certification, C++, Training, Jupyter, Nltk, Ai, Api, Python, Php, Programming, Django, Queries</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Logbook, Matplotlib, Html, Content, C, Tensorflow, Training, Analytics, Mysql, Sql, Communication, Numpy, Queries, Jupyter, Ai, Nltk, Programming, Research, System, Css, Rest, Certification, Php, Pandas, Testing, Technical, Design, Python, C++, Apis, Database, Engineering, Django, Website, Javascript, Reports, Process, Analysis, Networking, Api</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Queries, Programming, Python, Process, Networking, Django, Nltk, Communication, Analysis, C, Css, Rest, Sql, Ai, C++, Matplotlib, Certification, System, Mysql, Technical, Reports, Website, Tensorflow, Testing, Database, Logbook, Php, Design, Apis, Content, Research, Jupyter, Javascript, Html, Numpy, Training, Engineering, Api, Analytics, Pandas</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Queries, Programming, Python, Process, Networking, Django, Nltk, Communication, Analysis, C, Css, Rest, Sql, Ai, C++, Matplotlib, Certification, System, Mysql, Technical, Reports, Website, Tensorflow, Testing, Database, Logbook, Php, Design, Apis, Content, Research, Jupyter, Javascript, Html, Numpy, Training, Engineering, Api, Analytics, Pandas</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Queries, Programming, Python, Process, Networking, Nltk, Analysis, C, Css, Sql, C++, Matplotlib, Certification, Mysql, Technical, Reports, Mining, Spacy, Website, Tensorflow, Database, Warehouse, Php, Logbook, Design, Content, Research, Jupyter, Javascript, Html, Numpy, Training, Engineering, Analytics, Pandas</t>
         </is>
       </c>
     </row>
@@ -591,6 +832,206 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mobile No.</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Skills</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>R, C, P</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mobile No.</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Skills</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>9423627124</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Editing, Programming, English, Python, Css, Content, Training, Networking, Research, Database, Engineering, Php, Website, Analysis, Tensorflow, C, Html, Technical, Writing, Video</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mobile No.</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Skills</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>9423627124</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Html, Programming, Website, Engineering, Python, Technical, Database, Editing, Video, Training, English, Php, Analysis, Networking, Writing, C, Tensorflow, Content, Research, Css</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>athale20comp@student.mes.ac.in</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Design, Html, Css, System, Php, Java, Programming, Engineering, Python, Flask, Django, Javascript, C</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>pranjupolawar27@gmail.com</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>7058168004</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Github, Design, English, Html, Css, Website, Programming, Engineering, Python, Technical, Algorithms, Sql, Testing, C</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>maheshwariudhayan1@gmail.com</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>9975635803</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>International, Github, Content, English, Design, Html, Css, Website, Programming, Engineering, Python, Technical, Algorithms, Networking, Editing, Testing, Photography, C</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -660,7 +1101,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -730,7 +1171,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -754,6 +1195,692 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mobile No.</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Skills</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Mysql, Sql, Pandas, Nltk, Warehouse, Process, Php, Jupyter, Matplotlib, Engineering, Mining, Python, Analytics, Spacy, Logbook, Certification, Numpy, Analysis, Networking, Queries, Content, Reports, Css, Research, C, Html, Database, Technical, Design, Training, Programming, C++, Tensorflow, Javascript, Website</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Mysql, Sql, Pandas, Nltk, Warehouse, Process, Php, Jupyter, Matplotlib, Engineering, Mining, Python, Analytics, Spacy, Logbook, Certification, Numpy, Analysis, Networking, Queries, Content, Reports, Css, Research, C, Html, Database, Technical, Design, Training, Programming, C++, Tensorflow, Javascript, Website</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Numpy, Analysis, Nltk, Design, Sql, Logbook, Research, Mysql, Python, Html, Engineering, Jupyter, C++, Certification, Queries, Php, Process, Spacy, Technical, Training, Content, Matplotlib, Networking, C, Database, Css, Javascript, Tensorflow, Analytics, Website, Pandas, Mining, Programming, Warehouse, Reports</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Numpy, Analysis, Nltk, Design, Sql, Logbook, Research, Mysql, Python, Html, Engineering, Jupyter, C++, Certification, Queries, Php, Process, Spacy, Technical, Training, Content, Matplotlib, Networking, C, Database, Css, Javascript, Tensorflow, Analytics, Website, Pandas, Mining, Programming, Warehouse, Reports</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Numpy, Analysis, Nltk, Design, Sql, Logbook, Research, Mysql, Python, Html, Engineering, Jupyter, C++, Certification, Queries, Php, Process, Spacy, Technical, Training, Content, Matplotlib, Networking, C, Database, Css, Javascript, Tensorflow, Analytics, Website, Pandas, Mining, Programming, Warehouse, Reports</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Numpy, Analysis, Nltk, Design, Sql, Logbook, Research, Mysql, Python, Html, Engineering, Jupyter, C++, Certification, Queries, Php, Process, Spacy, Technical, Training, Content, Matplotlib, Networking, C, Database, Css, Javascript, Tensorflow, Analytics, Website, Pandas, Mining, Programming, Warehouse, Reports</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Numpy, Analysis, Nltk, Design, Sql, Logbook, Research, Mysql, Python, Html, Engineering, Jupyter, C++, Certification, Queries, Php, Process, Spacy, Technical, Training, Content, Matplotlib, Networking, C, Database, Css, Javascript, Tensorflow, Analytics, Website, Pandas, Mining, Programming, Warehouse, Reports</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Numpy, Analysis, Nltk, Design, Sql, Logbook, Research, Mysql, Python, Html, Engineering, Jupyter, C++, Certification, Queries, Php, Process, Spacy, Technical, Training, Content, Matplotlib, Networking, C, Database, Css, Javascript, Tensorflow, Analytics, Website, Pandas, Mining, Programming, Warehouse, Reports</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Numpy, Analysis, Nltk, Design, Sql, Logbook, Research, Mysql, Python, Html, Engineering, Jupyter, C++, Certification, Queries, Php, Process, Spacy, Technical, Training, Content, Matplotlib, Networking, C, Database, Css, Javascript, Tensorflow, Analytics, Website, Pandas, Mining, Programming, Warehouse, Reports</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Numpy, Analysis, Nltk, Design, Sql, Logbook, Research, Mysql, Python, Html, Engineering, Jupyter, C++, Certification, Queries, Php, Process, Spacy, Technical, Training, Content, Matplotlib, Networking, C, Database, Css, Javascript, Tensorflow, Analytics, Website, Pandas, Mining, Programming, Warehouse, Reports</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Numpy, Analysis, Nltk, Design, Sql, Logbook, Research, Mysql, Python, Html, Engineering, Jupyter, C++, Certification, Queries, Php, Process, Spacy, Technical, Training, Content, Matplotlib, Networking, C, Database, Css, Javascript, Tensorflow, Analytics, Website, Pandas, Mining, Programming, Warehouse, Reports</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Design, Engineering, Mysql, Pandas, C, Logbook, Reports, Php, Training, Programming, Analysis, Python, Database, Website, Numpy, Networking, Sql, Technical, Process, C++, Mining, Jupyter, Warehouse, Spacy, Nltk, Research, Analytics, Matplotlib, Javascript, Certification, Css, Html, Content, Tensorflow, Queries</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Jupyter, Pandas, Reports, Design, Logbook, Mysql, Mining, Python, Analytics, Process, Research, Css, Numpy, Certification, Php, Programming, Analysis, Content, Engineering, Sql, Training, C, Website, Networking, Warehouse, Technical, Matplotlib, Queries, Database, Nltk, C++, Html, Javascript, Tensorflow, Spacy</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Jupyter, Pandas, Reports, Design, Logbook, Mysql, Mining, Python, Analytics, Process, Research, Css, Numpy, Certification, Php, Programming, Analysis, Content, Engineering, Sql, Training, C, Website, Networking, Warehouse, Technical, Matplotlib, Queries, Database, Nltk, C++, Html, Javascript, Tensorflow, Spacy</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Css, Certification, Training, Logbook, Programming, Pandas, Analysis, Mysql, Website, Jupyter, Database, Python, C++, Content, Html, Reports, Engineering, Nltk, Spacy, Queries, Tensorflow, Numpy, Matplotlib, Process, Networking, Design, Sql, Technical, Javascript, Warehouse, C, Analytics, Php, Research, Mining</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Css, Certification, Training, Logbook, Programming, Pandas, Analysis, Mysql, Website, Jupyter, Database, Python, C++, Content, Html, Reports, Engineering, Nltk, Spacy, Queries, Tensorflow, Numpy, Matplotlib, Process, Networking, Design, Sql, Technical, Javascript, Warehouse, C, Analytics, Php, Research, Mining</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Numpy, Warehouse, Jupyter, Matplotlib, Design, Logbook, Javascript, Pandas, Reports, Sql, Nltk, Mining, Research, Technical, Html, C++, Content, C, Analytics, Mysql, Php, Networking, Python, Website, Programming, Training, Engineering, Queries, Process, Database, Certification, Tensorflow, Analysis, Spacy, Css</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Numpy, Warehouse, Jupyter, Matplotlib, Design, Logbook, Javascript, Pandas, Reports, Sql, Nltk, Mining, Research, Technical, Html, C++, Content, C, Analytics, Mysql, Php, Networking, Python, Website, Programming, Training, Engineering, Queries, Process, Database, Certification, Tensorflow, Analysis, Spacy, Css</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Certification, Warehouse, Engineering, Process, Javascript, Mining, Python, Tensorflow, Reports, Matplotlib, Pandas, Technical, Analysis, Mysql, Css, Html, Spacy, Website, C, Jupyter, Logbook, Numpy, Training, C++, Nltk, Research, Programming, Content, Design, Php, Queries, Analytics, Sql, Database, Networking</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Certification, Warehouse, Engineering, Process, Javascript, Mining, Python, Tensorflow, Reports, Matplotlib, Pandas, Technical, Analysis, Mysql, Css, Html, Spacy, Website, C, Jupyter, Logbook, Numpy, Training, C++, Nltk, Research, Programming, Content, Design, Php, Queries, Analytics, Sql, Database, Networking</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Certification, Warehouse, Engineering, Process, Javascript, Mining, Python, Tensorflow, Reports, Matplotlib, Pandas, Technical, Analysis, Mysql, Css, Html, Spacy, Website, C, Jupyter, Logbook, Numpy, Training, C++, Nltk, Research, Programming, Content, Design, Php, Queries, Analytics, Sql, Database, Networking</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Certification, Warehouse, Engineering, Process, Javascript, Mining, Python, Tensorflow, Reports, Matplotlib, Pandas, Technical, Analysis, Mysql, Css, Html, Spacy, Website, C, Jupyter, Logbook, Numpy, Training, C++, Nltk, Research, Programming, Content, Design, Php, Queries, Analytics, Sql, Database, Networking</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Certification, Warehouse, Engineering, Process, Javascript, Mining, Python, Tensorflow, Reports, Matplotlib, Pandas, Technical, Analysis, Mysql, Css, Html, Spacy, Website, C, Jupyter, Logbook, Numpy, Training, C++, Nltk, Research, Programming, Content, Design, Php, Queries, Analytics, Sql, Database, Networking</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mobile No.</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Skills</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Certification, Spacy, Reports, Analytics, Css, Database, Technical, Warehouse, Queries, Pandas, C, Mysql, Process, Nltk, Training, Engineering, Website, Content, Logbook, Matplotlib, Php, Research, C++, Html, Javascript, Design, Numpy, Sql, Programming, Mining, Jupyter, Networking, Tensorflow, Analysis, Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Certification, Spacy, Reports, Analytics, Css, Database, Technical, Warehouse, Queries, Pandas, C, Mysql, Process, Nltk, Training, Engineering, Website, Content, Logbook, Matplotlib, Php, Research, C++, Html, Javascript, Design, Numpy, Sql, Programming, Mining, Jupyter, Networking, Tensorflow, Analysis, Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Certification, Spacy, Reports, Analytics, Css, Database, Technical, Warehouse, Queries, Pandas, C, Mysql, Process, Nltk, Training, Engineering, Website, Content, Logbook, Matplotlib, Php, Research, C++, Html, Javascript, Design, Numpy, Sql, Programming, Mining, Jupyter, Networking, Tensorflow, Analysis, Python</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mobile No.</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Skills</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>C, Analytics, Database, Python, Engineering, Matplotlib, Java, Github, Access, Website, Javascript, Nltk, Django, Analysis, Training, Php, Css, Programming, Jupyter, Spacy, Numpy, Sql, Pandas, System, Algorithms, Html, Mysql, Technical, Testing, Seaborn</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>C, Analytics, Database, Python, Engineering, Matplotlib, Java, Github, Access, Website, Javascript, Nltk, Django, Analysis, Training, Php, Css, Programming, Jupyter, Spacy, Numpy, Sql, Pandas, System, Algorithms, Html, Mysql, Technical, Testing, Seaborn</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>C, Analytics, Database, Python, Engineering, Matplotlib, Java, Github, Access, Website, Javascript, Nltk, Django, Analysis, Training, Php, Css, Programming, Jupyter, Spacy, Numpy, Sql, Pandas, System, Algorithms, Html, Mysql, Technical, Testing, Seaborn</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Programming, Nltk, Java, Engineering, Database, Php, Sql, Jupyter, Javascript, Website, Django, Analytics, Spacy, Seaborn, Css, System, Html, Analysis, C, Python, Pandas, Access, Mysql, Algorithms, Technical, Matplotlib, Github, Testing, Numpy, Training</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Programming, Nltk, Java, Engineering, Database, Php, Sql, Jupyter, Javascript, Website, Django, Analytics, Spacy, Seaborn, Css, System, Html, Analysis, C, Python, Pandas, Access, Mysql, Algorithms, Technical, Matplotlib, Github, Testing, Numpy, Training</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Programming, Nltk, Java, Engineering, Database, Php, Sql, Jupyter, Javascript, Website, Django, Analytics, Spacy, Seaborn, Css, System, Html, Analysis, C, Python, Pandas, Access, Mysql, Algorithms, Technical, Matplotlib, Github, Testing, Numpy, Training</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Programming, Nltk, Java, Engineering, Database, Php, Sql, Jupyter, Javascript, Website, Django, Analytics, Spacy, Seaborn, Css, System, Html, Analysis, C, Python, Pandas, Access, Mysql, Algorithms, Technical, Matplotlib, Github, Testing, Numpy, Training</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Programming, Nltk, Java, Engineering, Database, Php, Sql, Jupyter, Javascript, Website, Django, Analytics, Spacy, Seaborn, Css, System, Html, Analysis, C, Python, Pandas, Access, Mysql, Algorithms, Technical, Matplotlib, Github, Testing, Numpy, Training</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1481,7 +2608,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1534,7 +2661,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1672,7 +2799,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1773,7 +2900,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1842,204 +2969,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Mobile No.</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Skills</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>R, C, P</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Mobile No.</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Skills</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>maheshkulkarni01121@gmail.com</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>9423627124</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Editing, Programming, English, Python, Css, Content, Training, Networking, Research, Database, Engineering, Php, Website, Analysis, Tensorflow, C, Html, Technical, Writing, Video</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Mobile No.</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Skills</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>maheshkulkarni01121@gmail.com</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>9423627124</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Html, Programming, Website, Engineering, Python, Technical, Database, Editing, Video, Training, English, Php, Analysis, Networking, Writing, C, Tensorflow, Content, Research, Css</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>athale20comp@student.mes.ac.in</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>+918605131403</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Design, Html, Css, System, Php, Java, Programming, Engineering, Python, Flask, Django, Javascript, C</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>pranjupolawar27@gmail.com</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>7058168004</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Github, Design, English, Html, Css, Website, Programming, Engineering, Python, Technical, Algorithms, Sql, Testing, C</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>maheshwariudhayan1@gmail.com</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>9975635803</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>International, Github, Content, English, Design, Html, Css, Website, Programming, Engineering, Python, Technical, Algorithms, Networking, Editing, Testing, Photography, C</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
made changes to ui
</commit_message>
<xml_diff>
--- a/ResumeSite/webapp/Extracted Data/Extracted.xlsx
+++ b/ResumeSite/webapp/Extracted Data/Extracted.xlsx
@@ -6,21 +6,23 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-04-09" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-04-07" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-04-05" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-02-24" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-02-23" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-10-30" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-10-22" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-10-21" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-10-19" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-10-16" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-10-04" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-09-01" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-08-31" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-08-29" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-04-13" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-04-10" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-04-09" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-04-07" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-04-05" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-02-24" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2024-02-23" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-10-30" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-10-22" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-10-21" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-10-19" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-10-16" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-10-04" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-09-01" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-08-31" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023-08-29" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -426,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,73 +476,48 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Bachelor of Technology, XII, X</t>
+          <t>XII, Bachelor of Technology, X</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Nltk, Html, Analytics, Spacy, Analysis, Engineering, Programming, Numpy, Matplotlib, C, Php, Testing, Jupyter, Algorithms, Sql, Database, Access, Github, Website, Django, Javascript, System, Technical, Css, Seaborn, Training, Pandas, Java, Mysql, Python</t>
+          <t>Technical, Numpy, Mysql, Java, Jupyter, Analytics, Html, Algorithms, Pandas, C, System, Spacy, Python, Testing, Seaborn, Engineering, Access, Django, Javascript, Php, Analysis, Nltk, Programming, Database, Sql, Website, Matplotlib, Training, Github, Css</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>thaleavanti2002@gmail.com</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>+918605131403</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology, XII, X</t>
-        </is>
-      </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Nltk, Html, Analytics, Spacy, Analysis, Engineering, Programming, Numpy, Matplotlib, C, Php, Testing, Jupyter, Algorithms, Sql, Database, Access, Github, Website, Django, Javascript, System, Technical, Css, Seaborn, Training, Pandas, Java, Mysql, Python</t>
+          <t>Brand, Health, Scheduling, Content, Editing, Design, Metrics, Writing, Engagement, Communication, Healthcare, Researching, Outreach, Reports</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>chithraedukulla@gmail.com</t>
+          <t>gargideshpande05@gmail.com</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>B.E</t>
+          <t>Bachelor of Technology</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Analysis, Design, Engineering, Sql, English, C, Technical, Java, Coding, Python</t>
+          <t>C, Programming, Css, Analytics, Technical, Python, Engineering, Sql, Html, Database, Biopython</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>thaleavanti2002@gmail.com</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>+918605131403</t>
-        </is>
-      </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>XII, Bachelor of Technology, X</t>
+          <t>Bachelor of Technology</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Django, Numpy, Javascript, Analytics, Jupyter, Training, Database, Css, Html, Access, Python, Pandas, Analysis, Engineering, Sql, System, Java, C, Mysql, Php, Website, Technical, Spacy, Programming, Nltk, Github, Algorithms, Matplotlib, Seaborn, Testing</t>
+          <t>Engineering</t>
         </is>
       </c>
     </row>
@@ -550,97 +527,72 @@
           <t>thaleavanti2002@gmail.com</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>+918605131403</t>
-        </is>
-      </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>XII, Bachelor of Technology, X</t>
+          <t>Bachelor of Engineering, BE</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Django, Numpy, Javascript, Analytics, Jupyter, Training, Database, Css, Html, Access, Python, Pandas, Analysis, Engineering, Sql, System, Java, C, Mysql, Php, Website, Technical, Spacy, Programming, Nltk, Github, Algorithms, Matplotlib, Seaborn, Testing</t>
+          <t>C, Programming, Analytics, Python, Analysis, Engineering</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>chithraedukulla@gmail.com</t>
+          <t>rajbharrohit212121@gmail.co</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>7021971</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>B.E</t>
+          <t>Bachelor of Engineering, BE</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Technical, Analysis, Design, Coding, Engineering, Sql, English, Python, Java, C</t>
+          <t>Marketing, Engineering, Mobile</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>thaleavanti2002@gmail.com</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>+918605131403</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>XII, X, Bachelor of Technology</t>
-        </is>
-      </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Engineering, Mysql, Training, Matplotlib, Css, Nltk, Github, Html, Spacy, Analytics, Database, Algorithms, Programming, Pandas, Django, System, Java, Website, Seaborn, Python, Php, Numpy, Sql, Analysis, Testing, Access, C, Jupyter, Javascript, Technical</t>
+          <t>Brand, Health, Scheduling, Content, Editing, Design, Metrics, Writing, Engagement, Communication, Healthcare, Researching, Outreach, Reports</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>thaleavanti2002@gmail.com</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>+918605131403</t>
+          <t>gargideshpande05@gmail.com</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>XII, X, Bachelor of Technology</t>
+          <t>Bachelor of Technology</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Engineering, Mysql, Training, Matplotlib, Css, Nltk, Github, Html, Spacy, Analytics, Database, Algorithms, Programming, Pandas, Django, System, Java, Website, Seaborn, Python, Php, Numpy, Sql, Analysis, Testing, Access, C, Jupyter, Javascript, Technical</t>
+          <t>C, Programming, Css, Analytics, Technical, Python, Engineering, Sql, Html, Database, Biopython</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>chithraedukulla@gmail.com</t>
-        </is>
-      </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>B.E</t>
+          <t>Bachelor of Technology</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Coding, Engineering, Design, Sql, Java, Analysis, C, Python, English, Technical</t>
+          <t>Engineering</t>
         </is>
       </c>
     </row>
@@ -650,202 +602,147 @@
           <t>thaleavanti2002@gmail.com</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>+918605131403</t>
-        </is>
-      </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>XII, X, Bachelor of Technology</t>
+          <t>Bachelor of Engineering, BE</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Engineering, Mysql, Training, Matplotlib, Css, Nltk, Github, Html, Spacy, Analytics, Database, Algorithms, Programming, Pandas, Django, System, Java, Website, Seaborn, Python, Php, Numpy, Sql, Analysis, Testing, Access, C, Jupyter, Javascript, Technical</t>
+          <t>C, Programming, Analytics, Python, Analysis, Engineering</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>thaleavanti2002@gmail.com</t>
+          <t>rajbharrohit212121@gmail.co</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>+918605131403</t>
+          <t>7021971</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>XII, X, Bachelor of Technology</t>
+          <t>Bachelor of Engineering, BE</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Engineering, Mysql, Training, Matplotlib, Css, Nltk, Github, Html, Spacy, Analytics, Database, Algorithms, Programming, Pandas, Django, System, Java, Website, Seaborn, Python, Php, Numpy, Sql, Analysis, Testing, Access, C, Jupyter, Javascript, Technical</t>
+          <t>Marketing, Engineering, Mobile</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>chithraedukulla@gmail.com</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>B.E</t>
-        </is>
-      </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Coding, Engineering, Design, Sql, Java, Analysis, C, Python, English, Technical</t>
+          <t>Healthcare, Brand, Content, Reports, Outreach, Metrics, Researching, Scheduling, Communication, Writing, Editing, Health, Engagement, Design</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>thaleavanti2002@gmail.com</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>+918605131403</t>
+          <t>gargideshpande05@gmail.com</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>X, Bachelor of Technology, XII</t>
+          <t>Bachelor of Technology</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Programming, Seaborn, Technical, Python, Javascript, Numpy, Php, Analytics, Training, Jupyter, Algorithms, Engineering, C, Nltk, Testing, Analysis, Sql, Mysql, Java, Access, System, Matplotlib, Website, Django, Database, Html, Spacy, Pandas, Css, Github</t>
+          <t>Sql, Programming, Analytics, Database, Technical, C, Biopython, Css, Python, Html, Engineering</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>thaleavanti2002@gmail.com</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>+918605131403</t>
-        </is>
-      </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>X, Bachelor of Technology, XII</t>
+          <t>Bachelor of Technology</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Programming, Seaborn, Technical, Python, Javascript, Numpy, Php, Analytics, Training, Jupyter, Algorithms, Engineering, C, Nltk, Testing, Analysis, Sql, Mysql, Java, Access, System, Matplotlib, Website, Django, Database, Html, Spacy, Pandas, Css, Github</t>
+          <t>Engineering</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>chithraedukulla@gmail.com</t>
+          <t>thaleavanti2002@gmail.com</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>B.E</t>
+          <t>Bachelor of Engineering, BE</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Design, Java, Technical, Engineering, C, Python, Analysis, English, Coding, Sql</t>
+          <t>Analysis, Programming, Analytics, C, Python, Engineering</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>thaleavanti2002@gmail.com</t>
+          <t>rajbharrohit212121@gmail.co</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>+918605131403</t>
+          <t>7021971</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Bachelor of Technology, XII, X</t>
+          <t>Bachelor of Engineering, BE</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Engineering, Mysql, Training, Spacy, Numpy, Matplotlib, Html, Analytics, Testing, Access, Django, Nltk, Jupyter, Python, System, Php, Technical, Analysis, Programming, Sql, Database, Java, Seaborn, Github, Css, Algorithms, Javascript, Website, Pandas, C</t>
+          <t>Mobile, Engineering, Marketing</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>thaleavanti2002@gmail.com</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>+918605131403</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology, XII, X</t>
-        </is>
-      </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Engineering, Mysql, Training, Spacy, Numpy, Matplotlib, Html, Analytics, Testing, Access, Django, Nltk, Jupyter, Python, System, Php, Technical, Analysis, Programming, Sql, Database, Java, Seaborn, Github, Css, Algorithms, Javascript, Website, Pandas, C</t>
+          <t>Outreach, Brand, Metrics, Communication, Health, Engagement, Content, Writing, Scheduling, Editing, Researching, Healthcare, Design, Reports</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>chithraedukulla@gmail.com</t>
+          <t>gargideshpande05@gmail.com</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>B.E</t>
+          <t>Bachelor of Technology</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Engineering, Technical, Analysis, Sql, Java, Design, English, Coding, Python, C</t>
+          <t>Technical, C, Sql, Html, Python, Css, Programming, Database, Analytics, Biopython, Engineering</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>thaleavanti2002@gmail.com</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>+918605131403</t>
-        </is>
-      </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>X, Bachelor of Technology, XII</t>
+          <t>Bachelor of Technology</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Programming, Css, Training, Mysql, Nltk, C, Technical, System, Jupyter, Pandas, Engineering, Analysis, Website, Python, Github, Java, Database, Html, Testing, Django, Php, Analytics, Javascript, Algorithms, Spacy, Sql, Access, Matplotlib, Seaborn, Numpy</t>
+          <t>Engineering</t>
         </is>
       </c>
     </row>
@@ -855,70 +752,50 @@
           <t>thaleavanti2002@gmail.com</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>+918605131403</t>
-        </is>
-      </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>X, Bachelor of Technology, XII</t>
+          <t>Bachelor of Engineering, BE</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Programming, Css, Training, Mysql, Nltk, C, Technical, System, Jupyter, Pandas, Analysis, Engineering, Website, Python, Github, Java, Database, Html, Testing, Django, Php, Analytics, Javascript, Algorithms, Spacy, Sql, Access, Matplotlib, Seaborn, Numpy</t>
+          <t>Analysis, C, Python, Programming, Analytics, Engineering</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>chithraedukulla@gmail.com</t>
+          <t>rajbharrohit212121@gmail.co</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>7021971</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>B.E</t>
+          <t>Bachelor of Engineering, BE</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Coding, Java, Design, English, Analysis, Engineering, Sql, C, Python, Technical</t>
+          <t>Mobile, Marketing, Engineering</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>mrunalkulkarni.2802@gmail.com</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Nltk, Research, Content, Warehouse, Design, Jupyter, Analytics, Queries, Logbook, Certification, Analysis, Database, Engineering, Training, C, Html, Process, Sql, Css, Tensorflow, Python, Programming, Reports, Mysql, Networking, Javascript, Technical, Website, Java, Mining, Php</t>
+          <t>Outreach, Brand, Metrics, Communication, Health, Engagement, Content, Writing, Scheduling, Editing, Researching, Healthcare, Design, Reports</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>maheshkulkarni01121@gmail.com</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>7715027944</t>
+          <t>gargideshpande05@gmail.com</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -928,65 +805,65 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Nltk, Research, Content, Warehouse, Design, Jupyter, Analytics, Matplotlib, Queries, Logbook, Certification, Analysis, Database, Engineering, Training, C, Html, Process, Sql, Css, C++, Tensorflow, Python, Programming, Mysql, Reports, Networking, Javascript, Technical, Website, Mining, Php</t>
+          <t>Technical, C, Sql, Html, Python, Css, Programming, Database, Analytics, Biopython, Engineering</t>
         </is>
       </c>
     </row>
     <row r="25">
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Outreach, Brand, Metrics, Engagement, Researching, Communication, Writing, Content, Reports, Design, Health, Scheduling, Editing, Healthcare</t>
+          <t>Engineering</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>mrunalkulkarni.2802@gmail.com</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>7715027944</t>
+          <t>thaleavanti2002@gmail.com</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Bachelor of Technology</t>
+          <t>Bachelor of Engineering, BE</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Technical, Warehouse, Process, Sql, Jupyter, Analytics, Javascript, Engineering, Database, Design, Reports, Certification, Php, Java, Queries, Networking, Tensorflow, Training, Programming, Research, Mysql, Python, Html, Mining, Content, Nltk, Css, C, Logbook, Analysis, Website</t>
+          <t>Analysis, C, Python, Programming, Analytics, Engineering</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>maheshkulkarni01121@gmail.com</t>
+          <t>rajbharrohit212121@gmail.co</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>7715027944</t>
+          <t>7021971</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Bachelor of Technology</t>
+          <t>Bachelor of Engineering, BE</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Technical, Warehouse, Process, Sql, Jupyter, Analytics, Javascript, Engineering, Database, Design, Reports, Certification, Php, Matplotlib, Queries, Networking, Tensorflow, Training, Programming, Research, Mysql, Python, C++, Html, Mining, Content, Nltk, Css, C, Logbook, Analysis, Website</t>
+          <t>Mobile, Marketing, Engineering</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="D28" t="inlineStr">
         <is>
-          <t>Design, Content, Researching, Scheduling, Reports, Healthcare, Editing, Writing, Communication, Metrics, Brand, Engagement, Outreach, Health</t>
+          <t>Outreach, Brand, Metrics, Communication, Health, Engagement, Content, Writing, Scheduling, Editing, Researching, Healthcare, Design, Reports</t>
         </is>
       </c>
     </row>
@@ -1003,7 +880,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Technical, Html, Engineering, Database, Biopython, Css, C, Sql, Python, Analytics, Programming</t>
+          <t>Technical, C, Sql, Html, Python, Css, Programming, Database, Analytics, Biopython, Engineering</t>
         </is>
       </c>
     </row>
@@ -1032,7 +909,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Engineering, C, Python, Analytics, Analysis, Programming</t>
+          <t>Analysis, C, Python, Programming, Analytics, Engineering</t>
         </is>
       </c>
     </row>
@@ -1054,41 +931,21 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Marketing, Engineering, Mobile</t>
+          <t>Mobile, Marketing, Engineering</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>sjstudy09@gmail.com</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>7063922</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Mathematics, Engineering, Content, C, Writing, Python, Strategy, Seo, Programming</t>
+          <t>Writing, Health, Design, Engagement, Scheduling, Outreach, Researching, Editing, Metrics, Communication, Reports, Brand, Healthcare, Content</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>mrunalkulkarni.2802@gmail.com</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>7715027944</t>
+          <t>gargideshpande05@gmail.com</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1098,21 +955,11 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Technical, Warehouse, Process, Sql, Jupyter, Analytics, Pandas, Javascript, Engineering, Database, Design, Reports, Certification, Php, Matplotlib, Queries, Networking, Tensorflow, Training, Programming, Spacy, Numpy, Research, Mysql, Python, C++, Html, Mining, Content, Nltk, Css, C, Logbook, Analysis, Website</t>
+          <t>Analytics, Python, Database, Programming, Biopython, Html, C, Technical, Sql, Engineering, Css</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>mrunalkulkarni.2802@gmail.com</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
       <c r="C35" t="inlineStr">
         <is>
           <t>Bachelor of Technology</t>
@@ -1120,58 +967,53 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Technical, Warehouse, Process, Sql, Jupyter, Analytics, Pandas, Javascript, Engineering, Database, Design, Reports, Certification, Php, Matplotlib, Queries, Networking, Tensorflow, Training, Programming, Spacy, Numpy, Research, Mysql, Python, C++, Html, Mining, Content, Nltk, Css, C, Logbook, Analysis, Website</t>
+          <t>Engineering</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>mrunalkulkarni.2802@gmail.com</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>7715027944</t>
+          <t>thaleavanti2002@gmail.com</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Bachelor of Technology</t>
+          <t>Bachelor of Engineering, BE</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Python, Design, Java, Database, Analysis, Html, Analytics, Nltk, Tensorflow, C, Research, Technical, Training, Queries, Website, Logbook, Php, Mining, Jupyter, Engineering, Warehouse, Mysql, Programming, Content, Process, Certification, Networking, Javascript, Css, Reports, Sql</t>
+          <t>Analytics, Python, Programming, C, Analysis, Engineering</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>maheshkulkarni01121@gmail.com</t>
+          <t>rajbharrohit212121@gmail.co</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>7715027944</t>
+          <t>7021971</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Bachelor of Technology</t>
+          <t>Bachelor of Engineering, BE</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Python, Design, Database, Analysis, Html, Analytics, Nltk, Tensorflow, C, Research, Technical, Training, Queries, Website, Logbook, Php, Mining, Jupyter, Engineering, C++, Warehouse, Mysql, Matplotlib, Programming, Content, Process, Certification, Networking, Javascript, Css, Reports, Sql</t>
+          <t>Engineering, Mobile, Marketing</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="D38" t="inlineStr">
         <is>
-          <t>Scheduling, Content, Design, Health, Outreach, Researching, Editing, Healthcare, Brand, Writing, Communication, Engagement, Reports, Metrics</t>
+          <t>Writing, Health, Design, Engagement, Scheduling, Outreach, Researching, Editing, Metrics, Communication, Reports, Brand, Healthcare, Content</t>
         </is>
       </c>
     </row>
@@ -1188,7 +1030,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Sql, Analytics, Python, C, Engineering, Biopython, Technical, Css, Database, Programming, Html</t>
+          <t>Analytics, Python, Database, Programming, Biopython, Html, C, Technical, Sql, Engineering, Css</t>
         </is>
       </c>
     </row>
@@ -1217,7 +1059,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Analytics, Python, C, Engineering, Analysis, Programming</t>
+          <t>Analytics, Python, Programming, C, Analysis, Engineering</t>
         </is>
       </c>
     </row>
@@ -1239,1390 +1081,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Mobile, Engineering, Marketing</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>sjstudy09@gmail.com</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>7063922</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>Mathematics, Content, Python, Strategy, C, Engineering, Seo, Writing, Programming</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>mrunalkulkarni.2802@gmail.com</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>Python, Design, Numpy, Database, Analysis, Html, Analytics, Nltk, Tensorflow, C, Research, Technical, Training, Queries, Website, Logbook, Php, Mining, Jupyter, Engineering, Pandas, C++, Warehouse, Matplotlib, Mysql, Programming, Content, Process, Certification, Networking, Javascript, Spacy, Css, Reports, Sql</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>mrunalkulkarni.2802@gmail.com</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>Python, Design, Numpy, Database, Analysis, Html, Analytics, Nltk, Tensorflow, C, Research, Technical, Training, Queries, Website, Logbook, Php, Mining, Jupyter, Engineering, Pandas, C++, Warehouse, Matplotlib, Mysql, Programming, Content, Process, Certification, Networking, Javascript, Spacy, Css, Reports, Sql</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>mrunalkulkarni.2802@gmail.com</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>Css, Queries, Database, Process, Analytics, Mysql, Warehouse, Design, C, Reports, Java, Training, Python, Logbook, Engineering, Analysis, Content, Programming, Website, Nltk, Research, Tensorflow, Javascript, Php, Certification, Mining, Sql, Jupyter, Technical, Html, Networking</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>maheshkulkarni01121@gmail.com</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>Css, Matplotlib, Queries, Database, Process, Analytics, Mysql, Warehouse, Design, C, C++, Reports, Training, Python, Logbook, Engineering, Analysis, Content, Programming, Website, Nltk, Research, Tensorflow, Javascript, Php, Certification, Mining, Sql, Jupyter, Technical, Html, Networking</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Editing, Outreach, Engagement, Content, Metrics, Health, Researching, Communication, Brand, Reports, Healthcare, Writing, Scheduling, Design</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>gargideshpande05@gmail.com</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Css, Biopython, Python, Engineering, C, Programming, Database, Sql, Analytics, Technical, Html</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>Engineering</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>thaleavanti2002@gmail.com</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>Bachelor of Engineering, BE</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>Python, Engineering, Analysis, C, Programming, Analytics</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>rajbharrohit212121@gmail.co</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>7021971</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>Bachelor of Engineering, BE</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>Engineering, Marketing, Mobile</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>sjstudy09@gmail.com</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>7063922</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>Strategy, Python, Engineering, Content, C, Programming, Writing, Mathematics, Seo</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>mrunalkulkarni.2802@gmail.com</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>Css, Pandas, Matplotlib, Queries, Database, Process, Analytics, Mysql, Warehouse, Design, Numpy, C, C++, Reports, Training, Python, Logbook, Engineering, Analysis, Content, Programming, Website, Nltk, Spacy, Research, Tensorflow, Javascript, Php, Certification, Mining, Sql, Jupyter, Technical, Html, Networking</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>mrunalkulkarni.2802@gmail.com</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>Css, Pandas, Matplotlib, Queries, Database, Process, Analytics, Mysql, Warehouse, Design, Numpy, C, C++, Reports, Training, Python, Logbook, Engineering, Analysis, Content, Programming, Website, Nltk, Spacy, Research, Tensorflow, Javascript, Php, Certification, Mining, Sql, Jupyter, Technical, Html, Networking</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>mrunalkulkarni.2802@gmail.com</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>Database, Design, Process, Sql, Css, C, Html, Content, Warehouse, Technical, Nltk, Javascript, Certification, Mining, Java, Programming, Php, Engineering, Analysis, Reports, Jupyter, Website, Research, Queries, Python, Tensorflow, Analytics, Logbook, Networking, Training, Mysql</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>maheshkulkarni01121@gmail.com</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>Database, Design, Process, Sql, Css, C, Html, Content, Warehouse, C++, Matplotlib, Technical, Nltk, Javascript, Certification, Mining, Programming, Php, Engineering, Analysis, Reports, Jupyter, Website, Research, Queries, Python, Tensorflow, Analytics, Logbook, Networking, Training, Mysql</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>Communication, Health, Metrics, Reports, Design, Editing, Brand, Researching, Outreach, Healthcare, Engagement, Scheduling, Writing, Content</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>gargideshpande05@gmail.com</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>Engineering, Database, Analytics, Technical, Sql, Css, C, Biopython, Html, Programming, Python</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>Engineering</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>thaleavanti2002@gmail.com</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>BE, Bachelor of Engineering</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>Engineering, Analysis, Analytics, C, Programming, Python</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>rajbharrohit212121@gmail.co</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>7021971</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>BE, Bachelor of Engineering</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>Mobile, Engineering, Marketing</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>sjstudy09@gmail.com</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>7063922</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>Engineering, Seo, C, Mathematics, Strategy, Programming, Writing, Python, Content</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>mrunalkulkarni.2802@gmail.com</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>Database, Design, Process, Sql, Css, C, Html, Content, Warehouse, C++, Matplotlib, Technical, Nltk, Numpy, Javascript, Certification, Mining, Programming, Php, Engineering, Analysis, Reports, Jupyter, Website, Research, Queries, Python, Tensorflow, Spacy, Analytics, Logbook, Networking, Training, Mysql, Pandas</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>mrunalkulkarni.2802@gmail.com</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>Database, Design, Process, Sql, Css, C, Html, Content, Warehouse, C++, Matplotlib, Technical, Nltk, Numpy, Javascript, Certification, Mining, Programming, Php, Engineering, Analysis, Reports, Jupyter, Website, Research, Queries, Python, Tensorflow, Spacy, Analytics, Logbook, Networking, Training, Mysql, Pandas</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>mrunalkulkarni.2802@gmail.com</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>Nltk, Tensorflow, Database, C, Networking, Website, Javascript, Warehouse, Design, Research, Java, Mysql, Logbook, Training, Queries, Python, Css, Jupyter, Programming, Content, Php, Engineering, Technical, Analysis, Html, Certification, Reports, Sql, Analytics, Mining, Process</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>maheshkulkarni01121@gmail.com</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>Tensorflow, Nltk, Database, C, Networking, Website, Javascript, Warehouse, Design, Research, Mysql, Logbook, Training, Queries, Python, Css, Jupyter, Programming, Content, Matplotlib, Php, Engineering, C++, Technical, Analysis, Html, Certification, Reports, Sql, Analytics, Mining, Process</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>Design, Communication, Brand, Writing, Scheduling, Health, Engagement, Outreach, Content, Researching, Metrics, Reports, Editing, Healthcare</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>gargideshpande05@gmail.com</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>Engineering, Technical, Database, Biopython, Programming, Css, Html, C, Sql, Analytics, Python</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>Engineering</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>thaleavanti2002@gmail.com</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>BE, Bachelor of Engineering</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>Engineering, Analysis, Programming, C, Analytics, Python</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>rajbharrohit212121@gmail.co</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>7021971</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>BE, Bachelor of Engineering</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
           <t>Engineering, Mobile, Marketing</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>sjstudy09@gmail.com</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>7063922</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>Engineering, Seo, Writing, Programming, Strategy, C, Content, Mathematics, Python</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>mrunalkulkarni.2802@gmail.com</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>Tensorflow, Nltk, Database, C, Networking, Website, Javascript, Warehouse, Design, Mining, Research, Mysql, Logbook, Training, Queries, Python, Css, Jupyter, Programming, Content, Matplotlib, Php, Engineering, C++, Spacy, Technical, Numpy, Analysis, Html, Certification, Reports, Sql, Analytics, Pandas, Process</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>mrunalkulkarni.2802@gmail.com</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>Tensorflow, Nltk, Database, C, Networking, Website, Javascript, Warehouse, Design, Mining, Research, Mysql, Logbook, Training, Queries, Python, Css, Jupyter, Programming, Content, Matplotlib, Php, Engineering, C++, Spacy, Technical, Numpy, Analysis, Html, Certification, Reports, Sql, Analytics, Pandas, Process</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>mrunalkulkarni.2802@gmail.com</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>Technical, Reports, Java, Javascript, Css, Training, Logbook, Nltk, Python, Programming, Mining, Html, Process, Tensorflow, Php, Analytics, Content, Networking, Database, Design, Website, C, Warehouse, Mysql, Research, Certification, Analysis, Engineering, Queries, Jupyter, Sql</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>maheshkulkarni01121@gmail.com</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>Technical, Reports, Javascript, Css, Training, Logbook, Nltk, Python, Programming, Mining, Html, Process, Tensorflow, Php, Analytics, Content, Networking, Database, Design, Website, C, Warehouse, Mysql, Research, Certification, Analysis, Engineering, Queries, Matplotlib, Jupyter, C++, Sql</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>Engagement, Reports, Brand, Healthcare, Health, Design, Researching, Writing, Outreach, Editing, Metrics, Scheduling, Content, Communication</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>gargideshpande05@gmail.com</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>Technical, Database, Html, Analytics, Engineering, Css, Sql, C, Python, Biopython, Programming</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>Engineering</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>thaleavanti2002@gmail.com</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>BE, Bachelor of Engineering</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>Analysis, Analytics, Engineering, C, Python, Programming</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>rajbharrohit212121@gmail.co</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>7021971</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>BE, Bachelor of Engineering</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>Engineering, Marketing, Mobile</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>sjstudy09@gmail.com</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>7063922</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>Writing, Engineering, Mathematics, C, Seo, Content, Strategy, Python, Programming</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>mrunalkulkarni.2802@gmail.com</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>Technical, Reports, Numpy, Javascript, Sql, Css, Training, Nltk, Logbook, Python, Programming, Mining, Html, Process, Tensorflow, Php, Analytics, Content, Networking, Database, Design, Website, C, Warehouse, Mysql, Research, Certification, Analysis, Engineering, Queries, Matplotlib, Jupyter, C++, Pandas, Spacy</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>mrunalkulkarni.2802@gmail.com</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>Technical, Reports, Numpy, Javascript, Sql, Css, Training, Nltk, Logbook, Python, Programming, Mining, Html, Process, Tensorflow, Php, Analytics, Content, Networking, Database, Design, Website, C, Warehouse, Mysql, Research, Certification, Analysis, Engineering, Queries, Matplotlib, Jupyter, C++, Pandas, Spacy</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>mrunalkulkarni.2802@gmail.com</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>Reports, Mining, C, Research, Certification, Sql, Technical, Analysis, Warehouse, Design, Html, Website, Jupyter, Python, Networking, Queries, Analytics, Programming, Mysql, Content, Php, Tensorflow, Javascript, Css, Java, Training, Database, Engineering, Logbook, Nltk, Process</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>maheshkulkarni01121@gmail.com</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>Reports, Mining, C, Research, Certification, Sql, Technical, Analysis, Warehouse, Design, Html, Website, Jupyter, Python, Networking, Queries, Analytics, Programming, Mysql, Content, Php, Tensorflow, Matplotlib, Css, C++, Javascript, Training, Database, Engineering, Logbook, Nltk, Process</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>Design, Brand, Researching, Reports, Metrics, Engagement, Scheduling, Writing, Communication, Healthcare, Editing, Outreach, Content, Health</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>gargideshpande05@gmail.com</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>Database, Html, Engineering, Biopython, Python, Css, C, Analytics, Programming, Sql, Technical</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>Engineering</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>thaleavanti2002@gmail.com</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>Bachelor of Engineering, BE</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>Analysis, Engineering, Python, C, Analytics, Programming</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>rajbharrohit212121@gmail.co</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>7021971</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>Bachelor of Engineering, BE</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>Mobile, Engineering, Marketing</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>sjstudy09@gmail.com</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>7063922</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t>Engineering, Seo, Python, Strategy, Writing, C, Programming, Mathematics, Content</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>mrunalkulkarni.2802@gmail.com</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t>Reports, Mining, C, Research, Certification, Sql, Technical, Analysis, Warehouse, Design, Html, Website, Jupyter, Python, Networking, Spacy, Pandas, Queries, Analytics, Programming, Mysql, Content, Php, Tensorflow, Matplotlib, Css, C++, Javascript, Training, Numpy, Database, Engineering, Logbook, Nltk, Process</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>mrunalkulkarni.2802@gmail.com</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t>Reports, Mining, C, Research, Certification, Sql, Technical, Analysis, Warehouse, Design, Html, Website, Jupyter, Python, Networking, Spacy, Pandas, Queries, Analytics, Programming, Mysql, Content, Php, Tensorflow, Matplotlib, Css, C++, Javascript, Training, Numpy, Database, Engineering, Logbook, Nltk, Process</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>thaleavanti2002@gmail.com</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>+918605131403</t>
-        </is>
-      </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>XII, Bachelor of Technology, X</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t>Java, Github, Database, Spacy, Analytics, System, Python, Seaborn, Jupyter, Sql, Testing, Php, Algorithms, Matplotlib, Html, Numpy, Mysql, Programming, C, Website, Access, Javascript, Pandas, Analysis, Nltk, Engineering, Technical, Css, Django, Training</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>thaleavanti2002@gmail.com</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>+918605131403</t>
-        </is>
-      </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>X, Bachelor of Technology, XII</t>
-        </is>
-      </c>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t>Nltk, Seaborn, Github, Numpy, Python, Training, Programming, Php, Sql, Jupyter, Analytics, Mysql, Java, Matplotlib, Engineering, System, Spacy, Pandas, C, Testing, Analysis, Access, Database, Javascript, Website, Technical, Django, Algorithms, Html, Css</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>thaleavanti2002@gmail.com</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>+918605131403</t>
-        </is>
-      </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>XII, X, Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t>Javascript, Database, Jupyter, Spacy, Access, Php, Analysis, Matplotlib, Django, Nltk, Algorithms, System, Technical, Pandas, Github, Programming, Analytics, Numpy, Engineering, Website, Training, Mysql, Java, Seaborn, Sql, Testing, Html, Python, C, Css</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>maheshkulkarni01121@gmail.com</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t>Queries, Javascript, Database, Jupyter, Networking, Research, Php, Reports, Analysis, Matplotlib, Nltk, Process, Technical, Tensorflow, Programming, Design, Analytics, Engineering, Website, Mining, Training, Logbook, Certification, Mysql, Warehouse, Sql, Html, Content, C++, Python, C, Css</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>thaleavanti2002@gmail.com</t>
-        </is>
-      </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t>Analysis, Programming, Database, Numpy, System, Python, Pandas, C</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>kpathare20comp@student.mes.ac.in</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>8767034204</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t>System, Javascript, Css, Health, Sql, English, C, Python, Content, Programming, Website, Writing, Engineering, Html</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>mrunalkulkarni.2802@gmail.com</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t>Process, Numpy, Spacy, Sql, C, Training, Certification, Analysis, Pandas, Database, Warehouse, Design, Php, Queries, Tensorflow, Html, Networking, Reports, Nltk, Mysql, C++, Programming, Mining, Content, Engineering, Javascript, Css, Matplotlib, Jupyter, Website, Analytics, Technical, Research, Logbook, Python</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>maheshkulkarni01121@gmail.com</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t>Process, Sql, C, Training, Certification, Analysis, Database, Warehouse, Design, Php, Queries, Tensorflow, Html, Networking, Reports, Nltk, Mysql, C++, Programming, Mining, Content, Engineering, Javascript, Css, Matplotlib, Jupyter, Website, Analytics, Technical, Research, Logbook, Python</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>mrunalkulkarni.2802@gmail.com</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t>Process, Numpy, Spacy, Sql, C, Training, Certification, Analysis, Pandas, Database, Warehouse, Design, Php, Queries, Tensorflow, Html, Networking, Reports, Nltk, Mysql, C++, Programming, Mining, Content, Engineering, Javascript, Css, Matplotlib, Jupyter, Website, Analytics, Technical, Research, Logbook, Python</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="D105" t="inlineStr">
-        <is>
-          <t>Editing, Reports, Outreach, Healthcare, Health, Design, Engagement, Scheduling, Researching, Content, Metrics, Writing, Brand, Communication</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>gargideshpande05@gmail.com</t>
-        </is>
-      </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t>Engineering, Database, Css, Sql, Biopython, Programming, C, Analytics, Technical, Python, Html</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t>Engineering</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>thaleavanti2002@gmail.com</t>
-        </is>
-      </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>Bachelor of Engineering, BE</t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>Analysis, C, Programming, Analytics, Engineering, Python</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>rajbharrohit212121@gmail.co</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>7021971</t>
-        </is>
-      </c>
-      <c r="C109" t="inlineStr">
-        <is>
-          <t>Bachelor of Engineering, BE</t>
-        </is>
-      </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t>Engineering, Marketing, Mobile</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>sjstudy09@gmail.com</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>7063922</t>
-        </is>
-      </c>
-      <c r="C110" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t>Mathematics, C, Programming, Strategy, Content, Writing, Seo, Engineering, Python</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>sjstudy09@gmail.com</t>
-        </is>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>7063922</t>
-        </is>
-      </c>
-      <c r="C111" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t>Mathematics, C, Programming, Strategy, Content, Writing, Seo, Engineering, Python</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="C112" t="inlineStr">
-        <is>
-          <t>Bachelor of Engineering, BE</t>
-        </is>
-      </c>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t>Engineering, C, .net, Java</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>sakshi20comp@student.mes.ac</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>257748273</t>
-        </is>
-      </c>
-      <c r="C113" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t>Engineering, Automation</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>athale20comp@student.mes.ac.in</t>
-        </is>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>+918605131403</t>
-        </is>
-      </c>
-      <c r="C114" t="inlineStr">
-        <is>
-          <t>XII, X</t>
-        </is>
-      </c>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t>System, Flask, Javascript, Css, Django, Design, Programming, C, Java, Php, Html, Engineering, Python</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>thaleavanti2002@gmail.com</t>
-        </is>
-      </c>
-      <c r="D115" t="inlineStr">
-        <is>
-          <t>Analysis, Pandas, Database, Numpy, C, Programming, System, Python</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>mrunalkulkarni.2802@gmail.com</t>
-        </is>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>7715027944</t>
-        </is>
-      </c>
-      <c r="C116" t="inlineStr">
-        <is>
-          <t>Bachelor of Technology</t>
-        </is>
-      </c>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t>Process, Numpy, Spacy, Sql, C, Training, Certification, Analysis, Pandas, Database, Warehouse, Design, Php, Queries, Tensorflow, Html, Networking, Reports, Nltk, Mysql, C++, Programming, Mining, Content, Engineering, Javascript, Css, Matplotlib, Jupyter, Website, Analytics, Technical, Research, Logbook, Python</t>
         </is>
       </c>
     </row>
@@ -2632,6 +1091,178 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mobile No.</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Skills</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>R, C, P</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>P, C, R</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>9423627124</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Html, Css, Website, English, Analysis, Training, Engineering, C, Editing, Php, Writing, Database, Video, Networking, Tensorflow, Research, Programming, Technical, Python, Content</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>9423627124</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Research, Html, Css, Php, Tensorflow, Networking, Database, Content, Website, Analysis, Python, C, Engineering, Training, Technical, English, Writing, Editing, Programming, Video</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>9423627124</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Writing, C, Css, Research, Editing, Php, Training, Database, Technical, English, Analysis, Tensorflow, Video, Html, Content, Website, Programming, Python, Engineering, Networking</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mobile No.</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Skills</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>C, P, R</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>C, R, P</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>C, R, P</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>C, R, P</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>C, R, P</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2674,7 +1305,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2727,7 +1358,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2831,7 +1462,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2901,7 +1532,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2971,7 +1602,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2995,6 +1626,2285 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mobile No.</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Eduaction</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Skills</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology, X, XII</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Sql, Analysis, Engineering, Training, Javascript, Github, Python, Seaborn, Numpy, Matplotlib, Analytics, Html, Website, Pandas, Technical, Jupyter, Mysql, Django, Access, Php, Algorithms, Nltk, Database, Programming, Spacy, Testing, System, Java, C, Css</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E116"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Mobile No.</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Eduaction</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Skills</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology, XII, X</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Nltk, Html, Analytics, Spacy, Analysis, Engineering, Programming, Numpy, Matplotlib, C, Php, Testing, Jupyter, Algorithms, Sql, Database, Access, Github, Website, Django, Javascript, System, Technical, Css, Seaborn, Training, Pandas, Java, Mysql, Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology, XII, X</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Nltk, Html, Analytics, Spacy, Analysis, Engineering, Programming, Numpy, Matplotlib, C, Php, Testing, Jupyter, Algorithms, Sql, Database, Access, Github, Website, Django, Javascript, System, Technical, Css, Seaborn, Training, Pandas, Java, Mysql, Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>chithraedukulla@gmail.com</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>B.E</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Analysis, Design, Engineering, Sql, English, C, Technical, Java, Coding, Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>XII, Bachelor of Technology, X</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Django, Numpy, Javascript, Analytics, Jupyter, Training, Database, Css, Html, Access, Python, Pandas, Analysis, Engineering, Sql, System, Java, C, Mysql, Php, Website, Technical, Spacy, Programming, Nltk, Github, Algorithms, Matplotlib, Seaborn, Testing</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>XII, Bachelor of Technology, X</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Django, Numpy, Javascript, Analytics, Jupyter, Training, Database, Css, Html, Access, Python, Pandas, Analysis, Engineering, Sql, System, Java, C, Mysql, Php, Website, Technical, Spacy, Programming, Nltk, Github, Algorithms, Matplotlib, Seaborn, Testing</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>chithraedukulla@gmail.com</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>B.E</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Technical, Analysis, Design, Coding, Engineering, Sql, English, Python, Java, C</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>XII, X, Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Engineering, Mysql, Training, Matplotlib, Css, Nltk, Github, Html, Spacy, Analytics, Database, Algorithms, Programming, Pandas, Django, System, Java, Website, Seaborn, Python, Php, Numpy, Sql, Analysis, Testing, Access, C, Jupyter, Javascript, Technical</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>XII, X, Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Engineering, Mysql, Training, Matplotlib, Css, Nltk, Github, Html, Spacy, Analytics, Database, Algorithms, Programming, Pandas, Django, System, Java, Website, Seaborn, Python, Php, Numpy, Sql, Analysis, Testing, Access, C, Jupyter, Javascript, Technical</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>chithraedukulla@gmail.com</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>B.E</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Coding, Engineering, Design, Sql, Java, Analysis, C, Python, English, Technical</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>XII, X, Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Engineering, Mysql, Training, Matplotlib, Css, Nltk, Github, Html, Spacy, Analytics, Database, Algorithms, Programming, Pandas, Django, System, Java, Website, Seaborn, Python, Php, Numpy, Sql, Analysis, Testing, Access, C, Jupyter, Javascript, Technical</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>XII, X, Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Engineering, Mysql, Training, Matplotlib, Css, Nltk, Github, Html, Spacy, Analytics, Database, Algorithms, Programming, Pandas, Django, System, Java, Website, Seaborn, Python, Php, Numpy, Sql, Analysis, Testing, Access, C, Jupyter, Javascript, Technical</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>chithraedukulla@gmail.com</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>B.E</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Coding, Engineering, Design, Sql, Java, Analysis, C, Python, English, Technical</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>X, Bachelor of Technology, XII</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Programming, Seaborn, Technical, Python, Javascript, Numpy, Php, Analytics, Training, Jupyter, Algorithms, Engineering, C, Nltk, Testing, Analysis, Sql, Mysql, Java, Access, System, Matplotlib, Website, Django, Database, Html, Spacy, Pandas, Css, Github</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>X, Bachelor of Technology, XII</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Programming, Seaborn, Technical, Python, Javascript, Numpy, Php, Analytics, Training, Jupyter, Algorithms, Engineering, C, Nltk, Testing, Analysis, Sql, Mysql, Java, Access, System, Matplotlib, Website, Django, Database, Html, Spacy, Pandas, Css, Github</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>chithraedukulla@gmail.com</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>B.E</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Design, Java, Technical, Engineering, C, Python, Analysis, English, Coding, Sql</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology, XII, X</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Engineering, Mysql, Training, Spacy, Numpy, Matplotlib, Html, Analytics, Testing, Access, Django, Nltk, Jupyter, Python, System, Php, Technical, Analysis, Programming, Sql, Database, Java, Seaborn, Github, Css, Algorithms, Javascript, Website, Pandas, C</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology, XII, X</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Engineering, Mysql, Training, Spacy, Numpy, Matplotlib, Html, Analytics, Testing, Access, Django, Nltk, Jupyter, Python, System, Php, Technical, Analysis, Programming, Sql, Database, Java, Seaborn, Github, Css, Algorithms, Javascript, Website, Pandas, C</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>chithraedukulla@gmail.com</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>B.E</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Engineering, Technical, Analysis, Sql, Java, Design, English, Coding, Python, C</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>X, Bachelor of Technology, XII</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Programming, Css, Training, Mysql, Nltk, C, Technical, System, Jupyter, Pandas, Engineering, Analysis, Website, Python, Github, Java, Database, Html, Testing, Django, Php, Analytics, Javascript, Algorithms, Spacy, Sql, Access, Matplotlib, Seaborn, Numpy</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>X, Bachelor of Technology, XII</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Programming, Css, Training, Mysql, Nltk, C, Technical, System, Jupyter, Pandas, Analysis, Engineering, Website, Python, Github, Java, Database, Html, Testing, Django, Php, Analytics, Javascript, Algorithms, Spacy, Sql, Access, Matplotlib, Seaborn, Numpy</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>chithraedukulla@gmail.com</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>B.E</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Coding, Java, Design, English, Analysis, Engineering, Sql, C, Python, Technical</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Nltk, Research, Content, Warehouse, Design, Jupyter, Analytics, Queries, Logbook, Certification, Analysis, Database, Engineering, Training, C, Html, Process, Sql, Css, Tensorflow, Python, Programming, Reports, Mysql, Networking, Javascript, Technical, Website, Java, Mining, Php</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Nltk, Research, Content, Warehouse, Design, Jupyter, Analytics, Matplotlib, Queries, Logbook, Certification, Analysis, Database, Engineering, Training, C, Html, Process, Sql, Css, C++, Tensorflow, Python, Programming, Mysql, Reports, Networking, Javascript, Technical, Website, Mining, Php</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Outreach, Brand, Metrics, Engagement, Researching, Communication, Writing, Content, Reports, Design, Health, Scheduling, Editing, Healthcare</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Technical, Warehouse, Process, Sql, Jupyter, Analytics, Javascript, Engineering, Database, Design, Reports, Certification, Php, Java, Queries, Networking, Tensorflow, Training, Programming, Research, Mysql, Python, Html, Mining, Content, Nltk, Css, C, Logbook, Analysis, Website</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Technical, Warehouse, Process, Sql, Jupyter, Analytics, Javascript, Engineering, Database, Design, Reports, Certification, Php, Matplotlib, Queries, Networking, Tensorflow, Training, Programming, Research, Mysql, Python, C++, Html, Mining, Content, Nltk, Css, C, Logbook, Analysis, Website</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Design, Content, Researching, Scheduling, Reports, Healthcare, Editing, Writing, Communication, Metrics, Brand, Engagement, Outreach, Health</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>gargideshpande05@gmail.com</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Technical, Html, Engineering, Database, Biopython, Css, C, Sql, Python, Analytics, Programming</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Bachelor of Engineering, BE</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Engineering, C, Python, Analytics, Analysis, Programming</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>rajbharrohit212121@gmail.co</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>7021971</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Bachelor of Engineering, BE</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Marketing, Engineering, Mobile</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>sjstudy09@gmail.com</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>7063922</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Mathematics, Engineering, Content, C, Writing, Python, Strategy, Seo, Programming</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Technical, Warehouse, Process, Sql, Jupyter, Analytics, Pandas, Javascript, Engineering, Database, Design, Reports, Certification, Php, Matplotlib, Queries, Networking, Tensorflow, Training, Programming, Spacy, Numpy, Research, Mysql, Python, C++, Html, Mining, Content, Nltk, Css, C, Logbook, Analysis, Website</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Technical, Warehouse, Process, Sql, Jupyter, Analytics, Pandas, Javascript, Engineering, Database, Design, Reports, Certification, Php, Matplotlib, Queries, Networking, Tensorflow, Training, Programming, Spacy, Numpy, Research, Mysql, Python, C++, Html, Mining, Content, Nltk, Css, C, Logbook, Analysis, Website</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Python, Design, Java, Database, Analysis, Html, Analytics, Nltk, Tensorflow, C, Research, Technical, Training, Queries, Website, Logbook, Php, Mining, Jupyter, Engineering, Warehouse, Mysql, Programming, Content, Process, Certification, Networking, Javascript, Css, Reports, Sql</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Python, Design, Database, Analysis, Html, Analytics, Nltk, Tensorflow, C, Research, Technical, Training, Queries, Website, Logbook, Php, Mining, Jupyter, Engineering, C++, Warehouse, Mysql, Matplotlib, Programming, Content, Process, Certification, Networking, Javascript, Css, Reports, Sql</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Scheduling, Content, Design, Health, Outreach, Researching, Editing, Healthcare, Brand, Writing, Communication, Engagement, Reports, Metrics</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>gargideshpande05@gmail.com</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Sql, Analytics, Python, C, Engineering, Biopython, Technical, Css, Database, Programming, Html</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Bachelor of Engineering, BE</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Analytics, Python, C, Engineering, Analysis, Programming</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>rajbharrohit212121@gmail.co</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>7021971</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Bachelor of Engineering, BE</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Mobile, Engineering, Marketing</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>sjstudy09@gmail.com</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>7063922</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Mathematics, Content, Python, Strategy, C, Engineering, Seo, Writing, Programming</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Python, Design, Numpy, Database, Analysis, Html, Analytics, Nltk, Tensorflow, C, Research, Technical, Training, Queries, Website, Logbook, Php, Mining, Jupyter, Engineering, Pandas, C++, Warehouse, Matplotlib, Mysql, Programming, Content, Process, Certification, Networking, Javascript, Spacy, Css, Reports, Sql</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Python, Design, Numpy, Database, Analysis, Html, Analytics, Nltk, Tensorflow, C, Research, Technical, Training, Queries, Website, Logbook, Php, Mining, Jupyter, Engineering, Pandas, C++, Warehouse, Matplotlib, Mysql, Programming, Content, Process, Certification, Networking, Javascript, Spacy, Css, Reports, Sql</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Css, Queries, Database, Process, Analytics, Mysql, Warehouse, Design, C, Reports, Java, Training, Python, Logbook, Engineering, Analysis, Content, Programming, Website, Nltk, Research, Tensorflow, Javascript, Php, Certification, Mining, Sql, Jupyter, Technical, Html, Networking</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Css, Matplotlib, Queries, Database, Process, Analytics, Mysql, Warehouse, Design, C, C++, Reports, Training, Python, Logbook, Engineering, Analysis, Content, Programming, Website, Nltk, Research, Tensorflow, Javascript, Php, Certification, Mining, Sql, Jupyter, Technical, Html, Networking</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Editing, Outreach, Engagement, Content, Metrics, Health, Researching, Communication, Brand, Reports, Healthcare, Writing, Scheduling, Design</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>gargideshpande05@gmail.com</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Css, Biopython, Python, Engineering, C, Programming, Database, Sql, Analytics, Technical, Html</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Bachelor of Engineering, BE</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Python, Engineering, Analysis, C, Programming, Analytics</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>rajbharrohit212121@gmail.co</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>7021971</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Bachelor of Engineering, BE</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Engineering, Marketing, Mobile</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>sjstudy09@gmail.com</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>7063922</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Strategy, Python, Engineering, Content, C, Programming, Writing, Mathematics, Seo</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Css, Pandas, Matplotlib, Queries, Database, Process, Analytics, Mysql, Warehouse, Design, Numpy, C, C++, Reports, Training, Python, Logbook, Engineering, Analysis, Content, Programming, Website, Nltk, Spacy, Research, Tensorflow, Javascript, Php, Certification, Mining, Sql, Jupyter, Technical, Html, Networking</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Css, Pandas, Matplotlib, Queries, Database, Process, Analytics, Mysql, Warehouse, Design, Numpy, C, C++, Reports, Training, Python, Logbook, Engineering, Analysis, Content, Programming, Website, Nltk, Spacy, Research, Tensorflow, Javascript, Php, Certification, Mining, Sql, Jupyter, Technical, Html, Networking</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Database, Design, Process, Sql, Css, C, Html, Content, Warehouse, Technical, Nltk, Javascript, Certification, Mining, Java, Programming, Php, Engineering, Analysis, Reports, Jupyter, Website, Research, Queries, Python, Tensorflow, Analytics, Logbook, Networking, Training, Mysql</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Database, Design, Process, Sql, Css, C, Html, Content, Warehouse, C++, Matplotlib, Technical, Nltk, Javascript, Certification, Mining, Programming, Php, Engineering, Analysis, Reports, Jupyter, Website, Research, Queries, Python, Tensorflow, Analytics, Logbook, Networking, Training, Mysql</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Communication, Health, Metrics, Reports, Design, Editing, Brand, Researching, Outreach, Healthcare, Engagement, Scheduling, Writing, Content</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>gargideshpande05@gmail.com</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Engineering, Database, Analytics, Technical, Sql, Css, C, Biopython, Html, Programming, Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>BE, Bachelor of Engineering</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Engineering, Analysis, Analytics, C, Programming, Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>rajbharrohit212121@gmail.co</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>7021971</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>BE, Bachelor of Engineering</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Mobile, Engineering, Marketing</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>sjstudy09@gmail.com</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>7063922</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Engineering, Seo, C, Mathematics, Strategy, Programming, Writing, Python, Content</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Database, Design, Process, Sql, Css, C, Html, Content, Warehouse, C++, Matplotlib, Technical, Nltk, Numpy, Javascript, Certification, Mining, Programming, Php, Engineering, Analysis, Reports, Jupyter, Website, Research, Queries, Python, Tensorflow, Spacy, Analytics, Logbook, Networking, Training, Mysql, Pandas</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Database, Design, Process, Sql, Css, C, Html, Content, Warehouse, C++, Matplotlib, Technical, Nltk, Numpy, Javascript, Certification, Mining, Programming, Php, Engineering, Analysis, Reports, Jupyter, Website, Research, Queries, Python, Tensorflow, Spacy, Analytics, Logbook, Networking, Training, Mysql, Pandas</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Nltk, Tensorflow, Database, C, Networking, Website, Javascript, Warehouse, Design, Research, Java, Mysql, Logbook, Training, Queries, Python, Css, Jupyter, Programming, Content, Php, Engineering, Technical, Analysis, Html, Certification, Reports, Sql, Analytics, Mining, Process</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Tensorflow, Nltk, Database, C, Networking, Website, Javascript, Warehouse, Design, Research, Mysql, Logbook, Training, Queries, Python, Css, Jupyter, Programming, Content, Matplotlib, Php, Engineering, C++, Technical, Analysis, Html, Certification, Reports, Sql, Analytics, Mining, Process</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Design, Communication, Brand, Writing, Scheduling, Health, Engagement, Outreach, Content, Researching, Metrics, Reports, Editing, Healthcare</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>gargideshpande05@gmail.com</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Engineering, Technical, Database, Biopython, Programming, Css, Html, C, Sql, Analytics, Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>BE, Bachelor of Engineering</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Engineering, Analysis, Programming, C, Analytics, Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>rajbharrohit212121@gmail.co</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>7021971</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>BE, Bachelor of Engineering</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Engineering, Mobile, Marketing</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>sjstudy09@gmail.com</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>7063922</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Engineering, Seo, Writing, Programming, Strategy, C, Content, Mathematics, Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Tensorflow, Nltk, Database, C, Networking, Website, Javascript, Warehouse, Design, Mining, Research, Mysql, Logbook, Training, Queries, Python, Css, Jupyter, Programming, Content, Matplotlib, Php, Engineering, C++, Spacy, Technical, Numpy, Analysis, Html, Certification, Reports, Sql, Analytics, Pandas, Process</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Tensorflow, Nltk, Database, C, Networking, Website, Javascript, Warehouse, Design, Mining, Research, Mysql, Logbook, Training, Queries, Python, Css, Jupyter, Programming, Content, Matplotlib, Php, Engineering, C++, Spacy, Technical, Numpy, Analysis, Html, Certification, Reports, Sql, Analytics, Pandas, Process</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Technical, Reports, Java, Javascript, Css, Training, Logbook, Nltk, Python, Programming, Mining, Html, Process, Tensorflow, Php, Analytics, Content, Networking, Database, Design, Website, C, Warehouse, Mysql, Research, Certification, Analysis, Engineering, Queries, Jupyter, Sql</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Technical, Reports, Javascript, Css, Training, Logbook, Nltk, Python, Programming, Mining, Html, Process, Tensorflow, Php, Analytics, Content, Networking, Database, Design, Website, C, Warehouse, Mysql, Research, Certification, Analysis, Engineering, Queries, Matplotlib, Jupyter, C++, Sql</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Engagement, Reports, Brand, Healthcare, Health, Design, Researching, Writing, Outreach, Editing, Metrics, Scheduling, Content, Communication</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>gargideshpande05@gmail.com</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Technical, Database, Html, Analytics, Engineering, Css, Sql, C, Python, Biopython, Programming</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>BE, Bachelor of Engineering</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Analysis, Analytics, Engineering, C, Python, Programming</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>rajbharrohit212121@gmail.co</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>7021971</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>BE, Bachelor of Engineering</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Engineering, Marketing, Mobile</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>sjstudy09@gmail.com</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>7063922</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Writing, Engineering, Mathematics, C, Seo, Content, Strategy, Python, Programming</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Technical, Reports, Numpy, Javascript, Sql, Css, Training, Nltk, Logbook, Python, Programming, Mining, Html, Process, Tensorflow, Php, Analytics, Content, Networking, Database, Design, Website, C, Warehouse, Mysql, Research, Certification, Analysis, Engineering, Queries, Matplotlib, Jupyter, C++, Pandas, Spacy</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Technical, Reports, Numpy, Javascript, Sql, Css, Training, Nltk, Logbook, Python, Programming, Mining, Html, Process, Tensorflow, Php, Analytics, Content, Networking, Database, Design, Website, C, Warehouse, Mysql, Research, Certification, Analysis, Engineering, Queries, Matplotlib, Jupyter, C++, Pandas, Spacy</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Reports, Mining, C, Research, Certification, Sql, Technical, Analysis, Warehouse, Design, Html, Website, Jupyter, Python, Networking, Queries, Analytics, Programming, Mysql, Content, Php, Tensorflow, Javascript, Css, Java, Training, Database, Engineering, Logbook, Nltk, Process</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Reports, Mining, C, Research, Certification, Sql, Technical, Analysis, Warehouse, Design, Html, Website, Jupyter, Python, Networking, Queries, Analytics, Programming, Mysql, Content, Php, Tensorflow, Matplotlib, Css, C++, Javascript, Training, Database, Engineering, Logbook, Nltk, Process</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Design, Brand, Researching, Reports, Metrics, Engagement, Scheduling, Writing, Communication, Healthcare, Editing, Outreach, Content, Health</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>gargideshpande05@gmail.com</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Database, Html, Engineering, Biopython, Python, Css, C, Analytics, Programming, Sql, Technical</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Bachelor of Engineering, BE</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Analysis, Engineering, Python, C, Analytics, Programming</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>rajbharrohit212121@gmail.co</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>7021971</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Bachelor of Engineering, BE</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Mobile, Engineering, Marketing</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>sjstudy09@gmail.com</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>7063922</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Engineering, Seo, Python, Strategy, Writing, C, Programming, Mathematics, Content</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Reports, Mining, C, Research, Certification, Sql, Technical, Analysis, Warehouse, Design, Html, Website, Jupyter, Python, Networking, Spacy, Pandas, Queries, Analytics, Programming, Mysql, Content, Php, Tensorflow, Matplotlib, Css, C++, Javascript, Training, Numpy, Database, Engineering, Logbook, Nltk, Process</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Reports, Mining, C, Research, Certification, Sql, Technical, Analysis, Warehouse, Design, Html, Website, Jupyter, Python, Networking, Spacy, Pandas, Queries, Analytics, Programming, Mysql, Content, Php, Tensorflow, Matplotlib, Css, C++, Javascript, Training, Numpy, Database, Engineering, Logbook, Nltk, Process</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>XII, Bachelor of Technology, X</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Java, Github, Database, Spacy, Analytics, System, Python, Seaborn, Jupyter, Sql, Testing, Php, Algorithms, Matplotlib, Html, Numpy, Mysql, Programming, C, Website, Access, Javascript, Pandas, Analysis, Nltk, Engineering, Technical, Css, Django, Training</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>X, Bachelor of Technology, XII</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Nltk, Seaborn, Github, Numpy, Python, Training, Programming, Php, Sql, Jupyter, Analytics, Mysql, Java, Matplotlib, Engineering, System, Spacy, Pandas, C, Testing, Analysis, Access, Database, Javascript, Website, Technical, Django, Algorithms, Html, Css</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>XII, X, Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Javascript, Database, Jupyter, Spacy, Access, Php, Analysis, Matplotlib, Django, Nltk, Algorithms, System, Technical, Pandas, Github, Programming, Analytics, Numpy, Engineering, Website, Training, Mysql, Java, Seaborn, Sql, Testing, Html, Python, C, Css</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Queries, Javascript, Database, Jupyter, Networking, Research, Php, Reports, Analysis, Matplotlib, Nltk, Process, Technical, Tensorflow, Programming, Design, Analytics, Engineering, Website, Mining, Training, Logbook, Certification, Mysql, Warehouse, Sql, Html, Content, C++, Python, C, Css</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Analysis, Programming, Database, Numpy, System, Python, Pandas, C</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>kpathare20comp@student.mes.ac.in</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>8767034204</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>System, Javascript, Css, Health, Sql, English, C, Python, Content, Programming, Website, Writing, Engineering, Html</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Process, Numpy, Spacy, Sql, C, Training, Certification, Analysis, Pandas, Database, Warehouse, Design, Php, Queries, Tensorflow, Html, Networking, Reports, Nltk, Mysql, C++, Programming, Mining, Content, Engineering, Javascript, Css, Matplotlib, Jupyter, Website, Analytics, Technical, Research, Logbook, Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>maheshkulkarni01121@gmail.com</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Process, Sql, C, Training, Certification, Analysis, Database, Warehouse, Design, Php, Queries, Tensorflow, Html, Networking, Reports, Nltk, Mysql, C++, Programming, Mining, Content, Engineering, Javascript, Css, Matplotlib, Jupyter, Website, Analytics, Technical, Research, Logbook, Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Process, Numpy, Spacy, Sql, C, Training, Certification, Analysis, Pandas, Database, Warehouse, Design, Php, Queries, Tensorflow, Html, Networking, Reports, Nltk, Mysql, C++, Programming, Mining, Content, Engineering, Javascript, Css, Matplotlib, Jupyter, Website, Analytics, Technical, Research, Logbook, Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Editing, Reports, Outreach, Healthcare, Health, Design, Engagement, Scheduling, Researching, Content, Metrics, Writing, Brand, Communication</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>gargideshpande05@gmail.com</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Engineering, Database, Css, Sql, Biopython, Programming, C, Analytics, Technical, Python, Html</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Engineering</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Bachelor of Engineering, BE</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Analysis, C, Programming, Analytics, Engineering, Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>rajbharrohit212121@gmail.co</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>7021971</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Bachelor of Engineering, BE</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Engineering, Marketing, Mobile</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>sjstudy09@gmail.com</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>7063922</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Mathematics, C, Programming, Strategy, Content, Writing, Seo, Engineering, Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>sjstudy09@gmail.com</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>7063922</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Mathematics, C, Programming, Strategy, Content, Writing, Seo, Engineering, Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Bachelor of Engineering, BE</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Engineering, C, .net, Java</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>sakshi20comp@student.mes.ac</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>257748273</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Engineering, Automation</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>athale20comp@student.mes.ac.in</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>+918605131403</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>XII, X</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>System, Flask, Javascript, Css, Django, Design, Programming, C, Java, Php, Html, Engineering, Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>thaleavanti2002@gmail.com</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Analysis, Pandas, Database, Numpy, C, Programming, System, Python</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>mrunalkulkarni.2802@gmail.com</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>7715027944</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Bachelor of Technology</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Process, Numpy, Spacy, Sql, C, Training, Certification, Analysis, Pandas, Database, Warehouse, Design, Php, Queries, Tensorflow, Html, Networking, Reports, Nltk, Mysql, C++, Programming, Mining, Content, Engineering, Javascript, Css, Matplotlib, Jupyter, Website, Analytics, Technical, Research, Logbook, Python</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3685,7 +4595,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3753,7 +4663,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3925,7 +4835,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4658,7 +5568,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4711,7 +5621,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4847,176 +5757,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Mobile No.</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Skills</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>R, C, P</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>P, C, R</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>maheshkulkarni01121@gmail.com</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>9423627124</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Html, Css, Website, English, Analysis, Training, Engineering, C, Editing, Php, Writing, Database, Video, Networking, Tensorflow, Research, Programming, Technical, Python, Content</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>maheshkulkarni01121@gmail.com</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>9423627124</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Research, Html, Css, Php, Tensorflow, Networking, Database, Content, Website, Analysis, Python, C, Engineering, Training, Technical, English, Writing, Editing, Programming, Video</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>maheshkulkarni01121@gmail.com</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>9423627124</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Writing, C, Css, Research, Editing, Php, Training, Database, Technical, English, Analysis, Tensorflow, Video, Html, Content, Website, Programming, Python, Engineering, Networking</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Mobile No.</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Skills</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>C, P, R</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>C, R, P</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>C, R, P</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>C, R, P</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>C, R, P</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>